<commit_message>
frs read in and eng inc plot tidied up
</commit_message>
<xml_diff>
--- a/data_output/comp_bandd_frsCTB.xlsx
+++ b/data_output/comp_bandd_frsCTB.xlsx
@@ -14,10 +14,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
-    <t>ctb_banddis</t>
-  </si>
-  <si>
-    <t>frs_banddis</t>
+    <t>comparison_df</t>
+  </si>
+  <si>
+    <t>V2</t>
   </si>
   <si>
     <t>banddis_diff</t>
@@ -115,10 +115,10 @@
         <v>23.940681250042367</v>
       </c>
       <c r="C2" t="n">
-        <v>20.567079290732686</v>
+        <v>20.646515533165406</v>
       </c>
       <c r="D2" t="n">
-        <v>3.3736019593096813</v>
+        <v>3.294165716876961</v>
       </c>
     </row>
     <row r="3">
@@ -129,10 +129,10 @@
         <v>19.522081660206993</v>
       </c>
       <c r="C3" t="n">
-        <v>18.492806958849116</v>
+        <v>18.564231738035264</v>
       </c>
       <c r="D3" t="n">
-        <v>1.0292747013578776</v>
+        <v>0.9578499221717287</v>
       </c>
     </row>
     <row r="4">
@@ -143,10 +143,10 @@
         <v>21.89281147899618</v>
       </c>
       <c r="C4" t="n">
-        <v>22.465707594513216</v>
+        <v>22.55247691015953</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.572896115517036</v>
+        <v>-0.6596654311633507</v>
       </c>
     </row>
     <row r="5">
@@ -157,10 +157,10 @@
         <v>15.607456603106993</v>
       </c>
       <c r="C5" t="n">
-        <v>17.029106724657076</v>
+        <v>17.094878253568428</v>
       </c>
       <c r="D5" t="n">
-        <v>-1.4216501215500834</v>
+        <v>-1.4874216504614353</v>
       </c>
     </row>
     <row r="6">
@@ -171,10 +171,10 @@
         <v>9.741197799161887</v>
       </c>
       <c r="C6" t="n">
-        <v>10.789561726329875</v>
+        <v>10.831234256926953</v>
       </c>
       <c r="D6" t="n">
-        <v>-1.0483639271679888</v>
+        <v>-1.0900364577650663</v>
       </c>
     </row>
     <row r="7">
@@ -185,10 +185,10 @@
         <v>5.171294850631392</v>
       </c>
       <c r="C7" t="n">
-        <v>6.0722649715623955</v>
+        <v>6.095717884130982</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.9009701209310039</v>
+        <v>-0.9244230334995907</v>
       </c>
     </row>
     <row r="8">
@@ -199,10 +199,10 @@
         <v>3.5297761021881007</v>
       </c>
       <c r="C8" t="n">
-        <v>3.747072599531616</v>
+        <v>3.7615449202350963</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.21729649734351542</v>
+        <v>-0.23176881804699567</v>
       </c>
     </row>
     <row r="9">
@@ -213,10 +213,10 @@
         <v>0.5947002556660862</v>
       </c>
       <c r="C9" t="n">
-        <v>0.45165607226497156</v>
+        <v>0.4534005037783375</v>
       </c>
       <c r="D9" t="n">
-        <v>0.14304418340111463</v>
+        <v>0.14129975188774868</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Just before it became PER YR
</commit_message>
<xml_diff>
--- a/data_output/comp_bandd_frsCTB.xlsx
+++ b/data_output/comp_bandd_frsCTB.xlsx
@@ -14,10 +14,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
-    <t>comparison_df</t>
-  </si>
-  <si>
-    <t>V2</t>
+    <t>ctb_banddis</t>
+  </si>
+  <si>
+    <t>frs_banddis</t>
   </si>
   <si>
     <t>banddis_diff</t>

</xml_diff>